<commit_message>
RTP caluclation was corrected.
</commit_message>
<xml_diff>
--- a/doc/Small-game-11-Aug-2017-1.xlsx
+++ b/doc/Small-game-11-Aug-2017-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="17">
   <si>
     <t xml:space="preserve">Drawn Balls:</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t xml:space="preserve">5 of 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combinations</t>
   </si>
   <si>
     <t xml:space="preserve">3 / 3</t>
@@ -172,12 +175,12 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="14.8469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -236,10 +239,13 @@
       <c r="G10" s="0" t="s">
         <v>10</v>
       </c>
+      <c r="I10" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>5000516</v>
@@ -259,10 +265,14 @@
       <c r="G11" s="0" t="n">
         <v>2999729</v>
       </c>
+      <c r="I11" s="0" t="n">
+        <f aca="false">COMBIN(3,3)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>0</v>
@@ -282,10 +292,14 @@
       <c r="G12" s="0" t="n">
         <v>11998778</v>
       </c>
+      <c r="I12" s="0" t="n">
+        <f aca="false">COMBIN(4,3)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0</v>
@@ -305,10 +319,14 @@
       <c r="G13" s="0" t="n">
         <v>30001200</v>
       </c>
+      <c r="I13" s="0" t="n">
+        <f aca="false">COMBIN(5,3)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -331,12 +349,12 @@
         <v>10</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" s="0" t="n">
         <f aca="false">5000516 / 10000000</f>
@@ -363,13 +381,13 @@
         <v>0.2999729</v>
       </c>
       <c r="I17" s="0" t="n">
-        <f aca="false">100 * SUM(E17:G17)</f>
+        <f aca="false">100 * SUM(E17:G17) / I11</f>
         <v>49.99484</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B18" s="0" t="n">
         <f aca="false">0 / 10000000</f>
@@ -396,13 +414,13 @@
         <v>1.1998778</v>
       </c>
       <c r="I18" s="0" t="n">
-        <f aca="false">100 * SUM(E18:G18)</f>
-        <v>199.9738</v>
+        <f aca="false">100 * SUM(E18:G18) / I12</f>
+        <v>49.99345</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B19" s="0" t="n">
         <f aca="false">0 / 10000000</f>
@@ -429,8 +447,8 @@
         <v>3.00012</v>
       </c>
       <c r="I19" s="0" t="n">
-        <f aca="false">100 * SUM(E19:G19)</f>
-        <v>499.97356</v>
+        <f aca="false">100 * SUM(E19:G19) / I13</f>
+        <v>49.997356</v>
       </c>
     </row>
   </sheetData>

</xml_diff>